<commit_message>
Remove unnecessary axis labels from chart radar example.
</commit_message>
<xml_diff>
--- a/test/perl_output/chart_radar.xlsx
+++ b/test/perl_output/chart_radar.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -259,24 +259,6 @@
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Test number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010002"/>
@@ -292,25 +274,8 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Sample length (mm)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010001"/>
         <c:crosses val="autoZero"/>
@@ -506,24 +471,6 @@
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Test number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020002"/>
@@ -539,25 +486,8 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Sample length (mm)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50020001"/>
         <c:crosses val="autoZero"/>
@@ -753,24 +683,6 @@
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Test number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50030002"/>
@@ -786,25 +698,8 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Sample length (mm)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50030001"/>
         <c:crosses val="autoZero"/>
@@ -862,13 +757,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -892,13 +787,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>